<commit_message>
actualizo repo a oct_2020
</commit_message>
<xml_diff>
--- a/informe_perdida_salarial/Entrada/base_informe_perdida.xlsx
+++ b/informe_perdida_salarial/Entrada/base_informe_perdida.xlsx
@@ -1,37 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Documents\Pablo\ATE-INDEC_perdida\Base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Documents\Pablo\ATE_INDEC\observatorio_indec\informe_perdida_salarial\Entrada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6641177-393C-470F-B9E6-5C6201F30E6D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884351FA-87BC-4473-AC06-E70B52CD4473}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
   <si>
     <t>periodo</t>
   </si>
@@ -1637,10 +1631,10 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A58" sqref="A58:A60"/>
+      <selection pane="bottomLeft" activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1699,7 +1693,7 @@
         <v>10190.89</v>
       </c>
       <c r="C3" s="3">
-        <f t="shared" ref="C3:C60" si="0">B3/$B$2*100</f>
+        <f t="shared" ref="C3:C61" si="0">B3/$B$2*100</f>
         <v>100</v>
       </c>
       <c r="D3" s="8">
@@ -3065,7 +3059,7 @@
         <v>449.10582897900957</v>
       </c>
       <c r="G55" s="5">
-        <f>C55/F55*100</f>
+        <f t="shared" ref="G55:G61" si="3">C55/F55*100</f>
         <v>69.770304615253636</v>
       </c>
     </row>
@@ -3090,7 +3084,7 @@
         <v>455.84241641369471</v>
       </c>
       <c r="G56" s="5">
-        <f>C56/F56*100</f>
+        <f t="shared" si="3"/>
         <v>68.739216369708018</v>
       </c>
     </row>
@@ -3115,7 +3109,7 @@
         <v>466.26565657228991</v>
       </c>
       <c r="G57" s="5">
-        <f>C57/F57*100</f>
+        <f t="shared" si="3"/>
         <v>67.202570145745739</v>
       </c>
     </row>
@@ -3140,7 +3134,7 @@
         <v>475.284141936222</v>
       </c>
       <c r="G58" s="5">
-        <f>C58/F58*100</f>
+        <f t="shared" si="3"/>
         <v>65.927405792882993</v>
       </c>
     </row>
@@ -3165,11 +3159,11 @@
         <v>488.11733828764051</v>
       </c>
       <c r="G59" s="5">
-        <f>C59/F59*100</f>
+        <f t="shared" si="3"/>
         <v>64.194094400077802</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="29">
         <v>44075</v>
       </c>
@@ -3190,8 +3184,33 @@
         <v>501.92803441756985</v>
       </c>
       <c r="G60" s="5">
-        <f>C60/F60*100</f>
+        <f t="shared" si="3"/>
         <v>62.427775186359781</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="29">
+        <v>44105</v>
+      </c>
+      <c r="B61" s="30">
+        <v>33886</v>
+      </c>
+      <c r="C61" s="3">
+        <f t="shared" si="0"/>
+        <v>332.5126657239947</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E61" t="s">
+        <v>2</v>
+      </c>
+      <c r="F61" s="5">
+        <v>520.89877085978026</v>
+      </c>
+      <c r="G61" s="5">
+        <f t="shared" si="3"/>
+        <v>63.834411660284594</v>
       </c>
     </row>
     <row r="1048575" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
actualizo script con proyecciones
</commit_message>
<xml_diff>
--- a/informe_perdida_salarial/Entrada/base_informe_perdida.xlsx
+++ b/informe_perdida_salarial/Entrada/base_informe_perdida.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Documents\Pablo\ATE_INDEC\observatorio_indec\informe_perdida_salarial\Entrada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11070BF2-288F-4ED4-86AC-74D19390C860}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDDC5B8-A177-44E9-93D1-9E648E55F933}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="D0" sheetId="1" r:id="rId1"/>
-    <sheet name="D5" sheetId="2" r:id="rId2"/>
+    <sheet name="E5" sheetId="3" r:id="rId2"/>
+    <sheet name="D5" sheetId="2" r:id="rId3"/>
+    <sheet name="C5" sheetId="5" r:id="rId4"/>
+    <sheet name="B5" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="18">
   <si>
     <t>periodo</t>
   </si>
@@ -62,6 +65,24 @@
   </si>
   <si>
     <t>inflacion_jun19_indice</t>
+  </si>
+  <si>
+    <t>y_e5_nominal</t>
+  </si>
+  <si>
+    <t>y_e5_evol</t>
+  </si>
+  <si>
+    <t>y_c5_nominal</t>
+  </si>
+  <si>
+    <t>y_c5_evol</t>
+  </si>
+  <si>
+    <t>y_b5_nominal</t>
+  </si>
+  <si>
+    <t>y_b5_evol</t>
   </si>
 </sst>
 </file>
@@ -400,7 +421,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -749,6 +770,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="310">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1065,7 +1123,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1167,6 +1225,11 @@
     <xf numFmtId="164" fontId="27" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="27" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="310">
     <cellStyle name="20% - Énfasis1 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1758,9 +1821,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1048566"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C71" sqref="C71"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3828125" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3377,12 +3440,610 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94470D22-5E2D-4DCA-827B-D838B6EA73C8}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="3" width="15.15234375" customWidth="1"/>
+    <col min="4" max="4" width="19.69140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="15.15234375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="35">
+        <v>43617</v>
+      </c>
+      <c r="B2" s="43">
+        <v>21905.5</v>
+      </c>
+      <c r="C2" s="3">
+        <f>B2/$B$2*100</f>
+        <v>100</v>
+      </c>
+      <c r="D2" s="38">
+        <v>225.53700000000001</v>
+      </c>
+      <c r="E2" s="5">
+        <f>C2/F2*100</f>
+        <v>100</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2/$D$2*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="36">
+        <v>43647</v>
+      </c>
+      <c r="B3" s="44">
+        <v>23377.84</v>
+      </c>
+      <c r="C3" s="3">
+        <f t="shared" ref="C3:C25" si="0">B3/$B$2*100</f>
+        <v>106.72132569446029</v>
+      </c>
+      <c r="D3" s="39">
+        <v>230.494</v>
+      </c>
+      <c r="E3" s="5">
+        <f t="shared" ref="E3:E25" si="1">C3/F3*100</f>
+        <v>104.42617869945201</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:F25" si="2">D3/$D$2*100</f>
+        <v>102.1978655386921</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="36">
+        <v>43678</v>
+      </c>
+      <c r="B4" s="44">
+        <v>24855.18</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" si="0"/>
+        <v>113.46547670676314</v>
+      </c>
+      <c r="D4" s="39">
+        <v>239.60769999999999</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" si="1"/>
+        <v>106.80234074286111</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="2"/>
+        <v>106.23875461675911</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="36">
+        <v>43709</v>
+      </c>
+      <c r="B5" s="44">
+        <v>24855.18</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="0"/>
+        <v>113.46547670676314</v>
+      </c>
+      <c r="D5" s="39">
+        <v>253.71019999999999</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" si="1"/>
+        <v>100.86572483098134</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="2"/>
+        <v>112.4916089156103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="36">
+        <v>43739</v>
+      </c>
+      <c r="B6" s="44">
+        <v>24855.18</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="0"/>
+        <v>113.46547670676314</v>
+      </c>
+      <c r="D6" s="39">
+        <v>262.06610000000001</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="1"/>
+        <v>97.649651061366711</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="2"/>
+        <v>116.19649990910584</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="36">
+        <v>43770</v>
+      </c>
+      <c r="B7" s="44">
+        <v>24855.18</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="0"/>
+        <v>113.46547670676314</v>
+      </c>
+      <c r="D7" s="39">
+        <v>273.2158</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="1"/>
+        <v>93.6646534351719</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="2"/>
+        <v>121.140123350049</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="36">
+        <v>43800</v>
+      </c>
+      <c r="B8" s="44">
+        <v>29855.18</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" si="0"/>
+        <v>136.29079454931409</v>
+      </c>
+      <c r="D8" s="39">
+        <v>283.44420000000002</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="1"/>
+        <v>108.44680162892256</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="2"/>
+        <v>125.67525505792842</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="36">
+        <v>43831</v>
+      </c>
+      <c r="B9" s="44">
+        <v>25908.28</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" si="0"/>
+        <v>118.27294515076122</v>
+      </c>
+      <c r="D9" s="39">
+        <v>289.82990000000001</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="1"/>
+        <v>92.036484953647772</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="2"/>
+        <v>128.50658650243639</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="36">
+        <v>43862</v>
+      </c>
+      <c r="B10" s="44">
+        <v>29961.38</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="0"/>
+        <v>136.77560430028987</v>
+      </c>
+      <c r="D10" s="39">
+        <v>295.666</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" si="1"/>
+        <v>104.33380729294026</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="2"/>
+        <v>131.09423287531536</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="36">
+        <v>43891</v>
+      </c>
+      <c r="B11" s="44">
+        <v>30961.38</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="0"/>
+        <v>141.3406678688001</v>
+      </c>
+      <c r="D11" s="39">
+        <v>305.55149999999998</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" si="1"/>
+        <v>104.32791267307009</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="2"/>
+        <v>135.47732744516418</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="36">
+        <v>43922</v>
+      </c>
+      <c r="B12" s="44">
+        <v>30961.38</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="0"/>
+        <v>141.3406678688001</v>
+      </c>
+      <c r="D12" s="39">
+        <v>310.12430000000001</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="1"/>
+        <v>102.78959181568669</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="2"/>
+        <v>137.50484399455522</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="36">
+        <v>43952</v>
+      </c>
+      <c r="B13" s="44">
+        <v>30961.38</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" si="0"/>
+        <v>141.3406678688001</v>
+      </c>
+      <c r="D13" s="39">
+        <v>314.90870000000001</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="1"/>
+        <v>101.22791211905408</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="2"/>
+        <v>139.62618107006833</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="36">
+        <v>43983</v>
+      </c>
+      <c r="B14" s="44">
+        <v>30961.38</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="0"/>
+        <v>141.3406678688001</v>
+      </c>
+      <c r="D14" s="39">
+        <v>321.97379999999998</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" si="1"/>
+        <v>99.006658955249065</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="2"/>
+        <v>142.75874911876986</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="36">
+        <v>44013</v>
+      </c>
+      <c r="B15" s="44">
+        <v>30961.38</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="0"/>
+        <v>141.3406678688001</v>
+      </c>
+      <c r="D15" s="39">
+        <v>328.20139999999998</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="1"/>
+        <v>97.128014106964713</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="2"/>
+        <v>145.51998120042387</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="36">
+        <v>44044</v>
+      </c>
+      <c r="B16" s="44">
+        <v>30961.38</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="0"/>
+        <v>141.3406678688001</v>
+      </c>
+      <c r="D16" s="39">
+        <v>337.06319999999999</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" si="1"/>
+        <v>94.574400910943609</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="2"/>
+        <v>149.44918128732758</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="36">
+        <v>44075</v>
+      </c>
+      <c r="B17" s="44">
+        <v>30961.38</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="0"/>
+        <v>141.3406678688001</v>
+      </c>
+      <c r="D17" s="39">
+        <v>346.6207</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="1"/>
+        <v>91.966666183310934</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="2"/>
+        <v>153.68684517396258</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="36">
+        <v>44105</v>
+      </c>
+      <c r="B18" s="44">
+        <v>32847.979999999996</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="0"/>
+        <v>149.95311679715138</v>
+      </c>
+      <c r="D18" s="39">
+        <v>359.65699999999998</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="1"/>
+        <v>94.033971542550631</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" si="2"/>
+        <v>159.46696107512292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="36">
+        <v>44136</v>
+      </c>
+      <c r="B19" s="44">
+        <v>32847.979999999996</v>
+      </c>
+      <c r="C19" s="3">
+        <f t="shared" si="0"/>
+        <v>149.95311679715138</v>
+      </c>
+      <c r="D19" s="39">
+        <v>371.02109999999999</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="1"/>
+        <v>91.153781019675506</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="2"/>
+        <v>164.50564652363028</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="36">
+        <v>44166</v>
+      </c>
+      <c r="B20" s="44">
+        <v>36847.979999999996</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" si="0"/>
+        <v>168.21337107119214</v>
+      </c>
+      <c r="D20" s="40">
+        <f>D19*1.03</f>
+        <v>382.15173299999998</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" si="1"/>
+        <v>99.275590806449287</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" si="2"/>
+        <v>169.44081591933917</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="36">
+        <v>44197</v>
+      </c>
+      <c r="B21" s="44">
+        <v>32847.979999999996</v>
+      </c>
+      <c r="C21" s="3">
+        <f t="shared" si="0"/>
+        <v>149.95311679715138</v>
+      </c>
+      <c r="D21" s="40">
+        <f t="shared" ref="D21:D22" si="3">D20*1.03</f>
+        <v>393.61628499</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" si="1"/>
+        <v>85.921181091220205</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" si="2"/>
+        <v>174.52404039691936</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="36">
+        <v>44228</v>
+      </c>
+      <c r="B22" s="44">
+        <v>33926.435199999993</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="0"/>
+        <v>154.87633334094173</v>
+      </c>
+      <c r="D22" s="40">
+        <f t="shared" si="3"/>
+        <v>405.42477353970003</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" si="1"/>
+        <v>86.157398048828213</v>
+      </c>
+      <c r="F22" s="3">
+        <f t="shared" si="2"/>
+        <v>179.75976160882695</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="36">
+        <v>44256</v>
+      </c>
+      <c r="B23" s="44">
+        <v>35544.117999999995</v>
+      </c>
+      <c r="C23" s="3">
+        <f t="shared" si="0"/>
+        <v>162.26115815662732</v>
+      </c>
+      <c r="D23" s="40">
+        <f>D22*1.02</f>
+        <v>413.53326901049405</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" si="1"/>
+        <v>88.495648523607855</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="2"/>
+        <v>183.35495684100349</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="36">
+        <v>44287</v>
+      </c>
+      <c r="B24" s="44">
+        <v>35544.120000000003</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" si="0"/>
+        <v>162.26116728675447</v>
+      </c>
+      <c r="D24" s="40">
+        <f>D23*1.02</f>
+        <v>421.80393439070394</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" si="1"/>
+        <v>86.76044461087244</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" si="2"/>
+        <v>187.02205597782356</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="37">
+        <v>44317</v>
+      </c>
+      <c r="B25" s="45">
+        <v>37701.030400000003</v>
+      </c>
+      <c r="C25" s="3">
+        <f t="shared" si="0"/>
+        <v>172.10760037433522</v>
+      </c>
+      <c r="D25" s="41">
+        <f>D24*1.02</f>
+        <v>430.24001307851802</v>
+      </c>
+      <c r="E25" s="5">
+        <f t="shared" si="1"/>
+        <v>90.220878313664613</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" si="2"/>
+        <v>190.76249709738002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AEC20B7-C21E-4A31-A031-B433C604527B}">
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3828125" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3997,4 +4658,1200 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37190119-5750-44A5-AE00-FCC009D42609}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="3" width="15.15234375" customWidth="1"/>
+    <col min="4" max="4" width="19.69140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="15.15234375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="35">
+        <v>43617</v>
+      </c>
+      <c r="B2" s="46">
+        <v>33599.99</v>
+      </c>
+      <c r="C2" s="3">
+        <f>B2/$B$2*100</f>
+        <v>100</v>
+      </c>
+      <c r="D2" s="38">
+        <v>225.53700000000001</v>
+      </c>
+      <c r="E2" s="5">
+        <f>C2/F2*100</f>
+        <v>100</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2/$D$2*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="36">
+        <v>43647</v>
+      </c>
+      <c r="B3" s="33">
+        <v>35858.36</v>
+      </c>
+      <c r="C3" s="3">
+        <f t="shared" ref="C3:C25" si="0">B3/$B$2*100</f>
+        <v>106.72134128611349</v>
+      </c>
+      <c r="D3" s="39">
+        <v>230.494</v>
+      </c>
+      <c r="E3" s="5">
+        <f t="shared" ref="E3:E25" si="1">C3/F3*100</f>
+        <v>104.42619395579138</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:F25" si="2">D3/$D$2*100</f>
+        <v>102.1978655386921</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="36">
+        <v>43678</v>
+      </c>
+      <c r="B4" s="33">
+        <v>38124.39</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" si="0"/>
+        <v>113.46548019805959</v>
+      </c>
+      <c r="D4" s="39">
+        <v>239.60769999999999</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" si="1"/>
+        <v>106.802344029135</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="2"/>
+        <v>106.23875461675911</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="36">
+        <v>43709</v>
+      </c>
+      <c r="B5" s="33">
+        <v>38124.39</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="0"/>
+        <v>113.46548019805959</v>
+      </c>
+      <c r="D5" s="39">
+        <v>253.71019999999999</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" si="1"/>
+        <v>100.86572793458744</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="2"/>
+        <v>112.4916089156103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="36">
+        <v>43739</v>
+      </c>
+      <c r="B6" s="33">
+        <v>38124.39</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="0"/>
+        <v>113.46548019805959</v>
+      </c>
+      <c r="D6" s="39">
+        <v>262.06610000000001</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="1"/>
+        <v>97.649654066015273</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="2"/>
+        <v>116.19649990910584</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="36">
+        <v>43770</v>
+      </c>
+      <c r="B7" s="33">
+        <v>38124.39</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="0"/>
+        <v>113.46548019805959</v>
+      </c>
+      <c r="D7" s="39">
+        <v>273.2158</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="1"/>
+        <v>93.664656317203338</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="2"/>
+        <v>121.140123350049</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="36">
+        <v>43800</v>
+      </c>
+      <c r="B8" s="33">
+        <v>43124.39</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" si="0"/>
+        <v>128.34643700786816</v>
+      </c>
+      <c r="D8" s="39">
+        <v>283.44420000000002</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="1"/>
+        <v>102.12546371893853</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="2"/>
+        <v>125.67525505792842</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="36">
+        <v>43831</v>
+      </c>
+      <c r="B9" s="33">
+        <v>39739.699999999997</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" si="0"/>
+        <v>118.27295186694995</v>
+      </c>
+      <c r="D9" s="39">
+        <v>289.82990000000001</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="1"/>
+        <v>92.03649017998589</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="2"/>
+        <v>128.50658650243639</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="36">
+        <v>43862</v>
+      </c>
+      <c r="B10" s="33">
+        <v>44355.01</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="0"/>
+        <v>132.00899762172548</v>
+      </c>
+      <c r="D10" s="39">
+        <v>295.666</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" si="1"/>
+        <v>100.69779175357026</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="2"/>
+        <v>131.09423287531536</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="36">
+        <v>43891</v>
+      </c>
+      <c r="B11" s="33">
+        <v>45356.01</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="0"/>
+        <v>134.98816517504918</v>
+      </c>
+      <c r="D11" s="39">
+        <v>305.55149999999998</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" si="1"/>
+        <v>99.638934219223501</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="2"/>
+        <v>135.47732744516418</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="36">
+        <v>43922</v>
+      </c>
+      <c r="B12" s="33">
+        <v>45356.01</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="0"/>
+        <v>134.98816517504918</v>
+      </c>
+      <c r="D12" s="39">
+        <v>310.12430000000001</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="1"/>
+        <v>98.169752609147579</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="2"/>
+        <v>137.50484399455522</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="36">
+        <v>43952</v>
+      </c>
+      <c r="B13" s="33">
+        <v>45356.01</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" si="0"/>
+        <v>134.98816517504918</v>
+      </c>
+      <c r="D13" s="39">
+        <v>314.90870000000001</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="1"/>
+        <v>96.678262013990292</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="2"/>
+        <v>139.62618107006833</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="36">
+        <v>43983</v>
+      </c>
+      <c r="B14" s="33">
+        <v>45356.01</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="0"/>
+        <v>134.98816517504918</v>
+      </c>
+      <c r="D14" s="39">
+        <v>321.97379999999998</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" si="1"/>
+        <v>94.556842230905332</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="2"/>
+        <v>142.75874911876986</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="36">
+        <v>44013</v>
+      </c>
+      <c r="B15" s="33">
+        <v>45356.01</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="0"/>
+        <v>134.98816517504918</v>
+      </c>
+      <c r="D15" s="39">
+        <v>328.20139999999998</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="1"/>
+        <v>92.762632362583048</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="2"/>
+        <v>145.51998120042387</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="36">
+        <v>44044</v>
+      </c>
+      <c r="B16" s="33">
+        <v>45356.01</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="0"/>
+        <v>134.98816517504918</v>
+      </c>
+      <c r="D16" s="39">
+        <v>337.06319999999999</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" si="1"/>
+        <v>90.323790342835011</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="2"/>
+        <v>149.44918128732758</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="36">
+        <v>44075</v>
+      </c>
+      <c r="B17" s="33">
+        <v>45356.01</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="0"/>
+        <v>134.98816517504918</v>
+      </c>
+      <c r="D17" s="39">
+        <v>346.6207</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="1"/>
+        <v>87.833259263180381</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="2"/>
+        <v>153.68684517396258</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="36">
+        <v>44105</v>
+      </c>
+      <c r="B18" s="33">
+        <v>48248.79</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="0"/>
+        <v>143.59763202310478</v>
+      </c>
+      <c r="D18" s="39">
+        <v>359.65699999999998</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="1"/>
+        <v>90.048516040546929</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" si="2"/>
+        <v>159.46696107512292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="36">
+        <v>44136</v>
+      </c>
+      <c r="B19" s="33">
+        <v>48248.79</v>
+      </c>
+      <c r="C19" s="3">
+        <f t="shared" si="0"/>
+        <v>143.59763202310478</v>
+      </c>
+      <c r="D19" s="39">
+        <v>371.02109999999999</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="1"/>
+        <v>87.290397051798351</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="2"/>
+        <v>164.50564652363028</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="36">
+        <v>44166</v>
+      </c>
+      <c r="B20" s="33">
+        <v>52248.79</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" si="0"/>
+        <v>155.50239747095165</v>
+      </c>
+      <c r="D20" s="40">
+        <f>D19*1.03</f>
+        <v>382.15173299999998</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" si="1"/>
+        <v>91.773871972486958</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" si="2"/>
+        <v>169.44081591933917</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="36">
+        <v>44197</v>
+      </c>
+      <c r="B21" s="33">
+        <v>48248.79</v>
+      </c>
+      <c r="C21" s="3">
+        <f t="shared" si="0"/>
+        <v>143.59763202310478</v>
+      </c>
+      <c r="D21" s="40">
+        <f t="shared" ref="D21:D22" si="3">D20*1.03</f>
+        <v>393.61628499</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" si="1"/>
+        <v>82.279571167686257</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" si="2"/>
+        <v>174.52404039691936</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="36">
+        <v>44228</v>
+      </c>
+      <c r="B22" s="33">
+        <v>49903.030400000003</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="0"/>
+        <v>148.52096801219287</v>
+      </c>
+      <c r="D22" s="40">
+        <f t="shared" si="3"/>
+        <v>405.42477353970003</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" si="1"/>
+        <v>82.621920880929707</v>
+      </c>
+      <c r="F22" s="3">
+        <f t="shared" si="2"/>
+        <v>179.75976160882695</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="36">
+        <v>44256</v>
+      </c>
+      <c r="B23" s="33">
+        <v>52384.391000000003</v>
+      </c>
+      <c r="C23" s="3">
+        <f t="shared" si="0"/>
+        <v>155.90597199582501</v>
+      </c>
+      <c r="D23" s="40">
+        <f>D22*1.02</f>
+        <v>413.53326901049405</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" si="1"/>
+        <v>85.029592153878397</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="2"/>
+        <v>183.35495684100349</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="36">
+        <v>44287</v>
+      </c>
+      <c r="B24" s="33">
+        <v>52384.39</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" si="0"/>
+        <v>155.90596901963366</v>
+      </c>
+      <c r="D24" s="40">
+        <f>D23*1.02</f>
+        <v>421.80393439070394</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" si="1"/>
+        <v>83.362343657541899</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" si="2"/>
+        <v>187.02205597782356</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="37">
+        <v>44317</v>
+      </c>
+      <c r="B25" s="47">
+        <v>55692.870799999997</v>
+      </c>
+      <c r="C25" s="3">
+        <f t="shared" si="0"/>
+        <v>165.75264099780981</v>
+      </c>
+      <c r="D25" s="41">
+        <f>D24*1.02</f>
+        <v>430.24001307851802</v>
+      </c>
+      <c r="E25" s="5">
+        <f t="shared" si="1"/>
+        <v>86.889532020120683</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" si="2"/>
+        <v>190.76249709738002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05CB5E3-7321-4B1A-A10D-B4E7E7141D9D}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="3" width="15.15234375" customWidth="1"/>
+    <col min="4" max="4" width="19.69140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="15.15234375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="35">
+        <v>43617</v>
+      </c>
+      <c r="B2" s="31">
+        <v>51070.400000000001</v>
+      </c>
+      <c r="C2" s="3">
+        <f>B2/$B$2*100</f>
+        <v>100</v>
+      </c>
+      <c r="D2" s="38">
+        <v>225.53700000000001</v>
+      </c>
+      <c r="E2" s="5">
+        <f>C2/F2*100</f>
+        <v>100</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2/$D$2*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="36">
+        <v>43647</v>
+      </c>
+      <c r="B3" s="32">
+        <v>54503.02</v>
+      </c>
+      <c r="C3" s="3">
+        <f t="shared" ref="C3:C25" si="0">B3/$B$2*100</f>
+        <v>106.72134935304989</v>
+      </c>
+      <c r="D3" s="39">
+        <v>230.494</v>
+      </c>
+      <c r="E3" s="5">
+        <f t="shared" ref="E3:E25" si="1">C3/F3*100</f>
+        <v>104.42620184924039</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:F25" si="2">D3/$D$2*100</f>
+        <v>102.1978655386921</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="36">
+        <v>43678</v>
+      </c>
+      <c r="B4" s="32">
+        <v>57947.28</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" si="0"/>
+        <v>113.46549077352046</v>
+      </c>
+      <c r="D4" s="39">
+        <v>239.60769999999999</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" si="1"/>
+        <v>106.80235398356348</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="2"/>
+        <v>106.23875461675911</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="36">
+        <v>43709</v>
+      </c>
+      <c r="B5" s="32">
+        <v>57947.28</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="0"/>
+        <v>113.46549077352046</v>
+      </c>
+      <c r="D5" s="39">
+        <v>253.71019999999999</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" si="1"/>
+        <v>100.8657373356983</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="2"/>
+        <v>112.4916089156103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="36">
+        <v>43739</v>
+      </c>
+      <c r="B6" s="32">
+        <v>57947.28</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="0"/>
+        <v>113.46549077352046</v>
+      </c>
+      <c r="D6" s="39">
+        <v>262.06610000000001</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="1"/>
+        <v>97.649663167374484</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="2"/>
+        <v>116.19649990910584</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="36">
+        <v>43770</v>
+      </c>
+      <c r="B7" s="32">
+        <v>57947.28</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="0"/>
+        <v>113.46549077352046</v>
+      </c>
+      <c r="D7" s="39">
+        <v>273.2158</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="1"/>
+        <v>93.664665047143984</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="2"/>
+        <v>121.140123350049</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="36">
+        <v>43800</v>
+      </c>
+      <c r="B8" s="33">
+        <v>62947.28</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" si="0"/>
+        <v>123.2558977411573</v>
+      </c>
+      <c r="D8" s="39">
+        <v>283.44420000000002</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="1"/>
+        <v>98.074913541527366</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="2"/>
+        <v>125.67525505792842</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="36">
+        <v>43831</v>
+      </c>
+      <c r="B9" s="32">
+        <v>60402.48</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" si="0"/>
+        <v>118.27297221090886</v>
+      </c>
+      <c r="D9" s="39">
+        <v>289.82990000000001</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="1"/>
+        <v>92.036506011049084</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="2"/>
+        <v>128.50658650243639</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="36">
+        <v>43862</v>
+      </c>
+      <c r="B10" s="32">
+        <v>62857.67</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="0"/>
+        <v>123.0804340674833</v>
+      </c>
+      <c r="D10" s="39">
+        <v>295.666</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" si="1"/>
+        <v>93.886993628885236</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="2"/>
+        <v>131.09423287531536</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="36">
+        <v>43891</v>
+      </c>
+      <c r="B11" s="32">
+        <v>62857.67</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="0"/>
+        <v>123.0804340674833</v>
+      </c>
+      <c r="D11" s="39">
+        <v>305.55149999999998</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" si="1"/>
+        <v>90.849470083694513</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="2"/>
+        <v>135.47732744516418</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="36">
+        <v>43922</v>
+      </c>
+      <c r="B12" s="32">
+        <v>62857.67</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="0"/>
+        <v>123.0804340674833</v>
+      </c>
+      <c r="D12" s="39">
+        <v>310.12430000000001</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="1"/>
+        <v>89.509889609675795</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="2"/>
+        <v>137.50484399455522</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="36">
+        <v>43952</v>
+      </c>
+      <c r="B13" s="32">
+        <v>62857.67</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" si="0"/>
+        <v>123.0804340674833</v>
+      </c>
+      <c r="D13" s="39">
+        <v>314.90870000000001</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="1"/>
+        <v>88.149968096397401</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="2"/>
+        <v>139.62618107006833</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="36">
+        <v>43983</v>
+      </c>
+      <c r="B14" s="32">
+        <v>62857.67</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="0"/>
+        <v>123.0804340674833</v>
+      </c>
+      <c r="D14" s="39">
+        <v>321.97379999999998</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" si="1"/>
+        <v>86.215685432410908</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="2"/>
+        <v>142.75874911876986</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="36">
+        <v>44013</v>
+      </c>
+      <c r="B15" s="32">
+        <v>62857.67</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="0"/>
+        <v>123.0804340674833</v>
+      </c>
+      <c r="D15" s="39">
+        <v>328.20139999999998</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="1"/>
+        <v>84.579748466270956</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="2"/>
+        <v>145.51998120042387</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="36">
+        <v>44044</v>
+      </c>
+      <c r="B16" s="32">
+        <v>62857.67</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="0"/>
+        <v>123.0804340674833</v>
+      </c>
+      <c r="D16" s="39">
+        <v>337.06319999999999</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" si="1"/>
+        <v>82.356044380632426</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="2"/>
+        <v>149.44918128732758</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="36">
+        <v>44075</v>
+      </c>
+      <c r="B17" s="32">
+        <v>62857.67</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="0"/>
+        <v>123.0804340674833</v>
+      </c>
+      <c r="D17" s="39">
+        <v>346.6207</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="1"/>
+        <v>80.085210889822747</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="2"/>
+        <v>153.68684517396258</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="36">
+        <v>44105</v>
+      </c>
+      <c r="B18" s="32">
+        <v>67256.08</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="0"/>
+        <v>131.69287884958803</v>
+      </c>
+      <c r="D18" s="39">
+        <v>359.65699999999998</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="1"/>
+        <v>82.583174572160516</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" si="2"/>
+        <v>159.46696107512292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="36">
+        <v>44136</v>
+      </c>
+      <c r="B19" s="32">
+        <v>67256.08</v>
+      </c>
+      <c r="C19" s="3">
+        <f t="shared" si="0"/>
+        <v>131.69287884958803</v>
+      </c>
+      <c r="D19" s="39">
+        <v>371.02109999999999</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="1"/>
+        <v>80.053713433277878</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="2"/>
+        <v>164.50564652363028</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="36">
+        <v>44166</v>
+      </c>
+      <c r="B20" s="32">
+        <v>67256.08</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" si="0"/>
+        <v>131.69287884958803</v>
+      </c>
+      <c r="D20" s="40">
+        <f>D19*1.03</f>
+        <v>382.15173299999998</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" si="1"/>
+        <v>77.722051876968806</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" si="2"/>
+        <v>169.44081591933917</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="36">
+        <v>44197</v>
+      </c>
+      <c r="B21" s="32">
+        <v>67256.08</v>
+      </c>
+      <c r="C21" s="3">
+        <f t="shared" si="0"/>
+        <v>131.69287884958803</v>
+      </c>
+      <c r="D21" s="40">
+        <f t="shared" ref="D21:D22" si="3">D20*1.03</f>
+        <v>393.61628499</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" si="1"/>
+        <v>75.458302793173601</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" si="2"/>
+        <v>174.52404039691936</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="36">
+        <v>44228</v>
+      </c>
+      <c r="B22" s="32">
+        <v>69770.386800000007</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="0"/>
+        <v>136.61609621228737</v>
+      </c>
+      <c r="D22" s="40">
+        <f t="shared" si="3"/>
+        <v>405.42477353970003</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" si="1"/>
+        <v>75.999264234437518</v>
+      </c>
+      <c r="F22" s="3">
+        <f t="shared" si="2"/>
+        <v>179.75976160882695</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="36">
+        <v>44256</v>
+      </c>
+      <c r="B23" s="32">
+        <v>73541.847000000009</v>
+      </c>
+      <c r="C23" s="3">
+        <f t="shared" si="0"/>
+        <v>144.00092225633637</v>
+      </c>
+      <c r="D23" s="40">
+        <f>D22*1.02</f>
+        <v>413.53326901049405</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" si="1"/>
+        <v>78.536694473554363</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="2"/>
+        <v>183.35495684100349</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="36">
+        <v>44287</v>
+      </c>
+      <c r="B24" s="32">
+        <v>73541.846999999994</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" si="0"/>
+        <v>144.00092225633634</v>
+      </c>
+      <c r="D24" s="40">
+        <f>D23*1.02</f>
+        <v>421.80393439070394</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" si="1"/>
+        <v>76.996759287798383</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" si="2"/>
+        <v>187.02205597782356</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="37">
+        <v>44317</v>
+      </c>
+      <c r="B25" s="34">
+        <v>78570.460599999991</v>
+      </c>
+      <c r="C25" s="3">
+        <f t="shared" si="0"/>
+        <v>153.847356981735</v>
+      </c>
+      <c r="D25" s="41">
+        <f>D24*1.02</f>
+        <v>430.24001307851802</v>
+      </c>
+      <c r="E25" s="5">
+        <f t="shared" si="1"/>
+        <v>80.648638659410793</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" si="2"/>
+        <v>190.76249709738002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
actualizo grafico y funcion a 2021
</commit_message>
<xml_diff>
--- a/informe_perdida_salarial/Entrada/base_informe_perdida.xlsx
+++ b/informe_perdida_salarial/Entrada/base_informe_perdida.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Documents\Pablo\ATE_INDEC\observatorio_indec\informe_perdida_salarial\Entrada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B2F929-0B70-4F77-AB44-068392CD67C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C341D54D-30C3-4D64-A90A-719C567BEB63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
   <si>
     <t>periodo</t>
   </si>
@@ -1123,7 +1123,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1230,6 +1230,12 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="310">
     <cellStyle name="20% - Énfasis1 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1823,7 +1829,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G64" sqref="G64"/>
+      <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3463,7 +3469,7 @@
         <v>66.524093864139928</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="29">
         <v>44197</v>
       </c>
@@ -3471,7 +3477,7 @@
         <v>33886</v>
       </c>
       <c r="C64" s="3">
-        <f t="shared" si="4"/>
+        <f>B64/$B$2*100</f>
         <v>332.5126657239947</v>
       </c>
       <c r="D64" s="11" t="s">
@@ -3484,8 +3490,33 @@
         <v>581.445831214652</v>
       </c>
       <c r="G64" s="5">
-        <f t="shared" si="5"/>
+        <f>C64/F64*100</f>
         <v>57.187212956599772</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="29">
+        <v>44228</v>
+      </c>
+      <c r="B65" s="48">
+        <v>35003.82</v>
+      </c>
+      <c r="C65" s="3">
+        <f>B65/$B$2*100</f>
+        <v>343.48148199028742</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F65" s="49">
+        <v>602.22602835797284</v>
+      </c>
+      <c r="G65" s="5">
+        <f>C65/F65*100</f>
+        <v>57.035309969385196</v>
       </c>
     </row>
     <row r="1048565" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>

</xml_diff>